<commit_message>
+added all staff form DS court case competition
</commit_message>
<xml_diff>
--- a/DS_competition/Paskaidrojumi-explanations.xlsx
+++ b/DS_competition/Paskaidrojumi-explanations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -825,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>